<commit_message>
replaced "piece" observations in dataset with English titles and adjusted code
</commit_message>
<xml_diff>
--- a/reception_analysis_data.xlsx
+++ b/reception_analysis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Zeldin\Documents\R stuff\R projects\dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276BC5F8-2822-4DCC-B7EB-D8E5C22A3114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0BDD9E-AEC2-44C1-85C1-DCDA2D80FDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{05090813-5714-498C-A2E7-B769A3723D8B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{05090813-5714-498C-A2E7-B769A3723D8B}"/>
   </bookViews>
   <sheets>
     <sheet name="all_docs_lowercase" sheetId="3" r:id="rId1"/>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="783">
   <si>
     <t>Article</t>
   </si>
@@ -3458,6 +3458,12 @@
   </si>
   <si>
     <t>piece</t>
+  </si>
+  <si>
+    <t>measures</t>
+  </si>
+  <si>
+    <t>mother</t>
   </si>
 </sst>
 </file>
@@ -4006,10 +4012,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD55270A-6EE4-4E29-A288-95E6364C6952}">
   <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4124,7 +4130,7 @@
         <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4171,7 +4177,7 @@
         <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4215,7 +4221,7 @@
         <v>26</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4265,7 +4271,7 @@
         <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4315,7 +4321,7 @@
         <v>26</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4365,7 +4371,7 @@
         <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4412,7 +4418,7 @@
         <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4459,7 +4465,7 @@
         <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4506,7 +4512,7 @@
         <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4556,7 +4562,7 @@
         <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4603,7 +4609,7 @@
         <v>26</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4647,7 +4653,7 @@
         <v>26</v>
       </c>
       <c r="P13" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4694,7 +4700,7 @@
         <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4744,7 +4750,7 @@
         <v>26</v>
       </c>
       <c r="P15" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4788,7 +4794,7 @@
         <v>26</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4835,7 +4841,7 @@
         <v>26</v>
       </c>
       <c r="P17" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4882,7 +4888,7 @@
         <v>26</v>
       </c>
       <c r="P18" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4929,7 +4935,7 @@
         <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4976,7 +4982,7 @@
         <v>26</v>
       </c>
       <c r="P20" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5023,7 +5029,7 @@
         <v>26</v>
       </c>
       <c r="P21" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5070,7 +5076,7 @@
         <v>26</v>
       </c>
       <c r="P22" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5117,7 +5123,7 @@
         <v>26</v>
       </c>
       <c r="P23" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5164,7 +5170,7 @@
         <v>26</v>
       </c>
       <c r="P24" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5214,7 +5220,7 @@
         <v>26</v>
       </c>
       <c r="P25" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5261,7 +5267,7 @@
         <v>26</v>
       </c>
       <c r="P26" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5305,7 +5311,7 @@
         <v>26</v>
       </c>
       <c r="P27" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5352,7 +5358,7 @@
         <v>26</v>
       </c>
       <c r="P28" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5396,7 +5402,7 @@
         <v>26</v>
       </c>
       <c r="P29" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5443,7 +5449,7 @@
         <v>26</v>
       </c>
       <c r="P30" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5490,7 +5496,7 @@
         <v>26</v>
       </c>
       <c r="P31" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5537,7 +5543,7 @@
         <v>26</v>
       </c>
       <c r="P32" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5584,7 +5590,7 @@
         <v>26</v>
       </c>
       <c r="P33" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5631,7 +5637,7 @@
         <v>26</v>
       </c>
       <c r="P34" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5681,7 +5687,7 @@
         <v>26</v>
       </c>
       <c r="P35" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5728,7 +5734,7 @@
         <v>26</v>
       </c>
       <c r="P36" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5775,7 +5781,7 @@
         <v>26</v>
       </c>
       <c r="P37" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5825,7 +5831,7 @@
         <v>26</v>
       </c>
       <c r="P38" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5875,7 +5881,7 @@
         <v>26</v>
       </c>
       <c r="P39" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5925,7 +5931,7 @@
         <v>26</v>
       </c>
       <c r="P40" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5972,7 +5978,7 @@
         <v>26</v>
       </c>
       <c r="P41" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6019,7 +6025,7 @@
         <v>26</v>
       </c>
       <c r="P42" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6066,7 +6072,7 @@
         <v>26</v>
       </c>
       <c r="P43" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6113,7 +6119,7 @@
         <v>26</v>
       </c>
       <c r="P44" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6163,7 +6169,7 @@
         <v>26</v>
       </c>
       <c r="P45" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6210,7 +6216,7 @@
         <v>26</v>
       </c>
       <c r="P46" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6254,7 +6260,7 @@
         <v>322</v>
       </c>
       <c r="P47" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6301,7 +6307,7 @@
         <v>322</v>
       </c>
       <c r="P48" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6342,7 +6348,7 @@
         <v>333</v>
       </c>
       <c r="P49" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6386,7 +6392,7 @@
         <v>333</v>
       </c>
       <c r="P50" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6430,7 +6436,7 @@
         <v>40</v>
       </c>
       <c r="P51" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6474,7 +6480,7 @@
         <v>355</v>
       </c>
       <c r="P52" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6521,7 +6527,7 @@
         <v>355</v>
       </c>
       <c r="P53" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6568,7 +6574,7 @@
         <v>355</v>
       </c>
       <c r="P54" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6615,7 +6621,7 @@
         <v>355</v>
       </c>
       <c r="P55" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6659,7 +6665,7 @@
         <v>355</v>
       </c>
       <c r="P56" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6706,7 +6712,7 @@
         <v>355</v>
       </c>
       <c r="P57" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6753,7 +6759,7 @@
         <v>355</v>
       </c>
       <c r="P58" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6800,7 +6806,7 @@
         <v>355</v>
       </c>
       <c r="P59" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6847,7 +6853,7 @@
         <v>355</v>
       </c>
       <c r="P60" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6894,7 +6900,7 @@
         <v>355</v>
       </c>
       <c r="P61" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6941,7 +6947,7 @@
         <v>355</v>
       </c>
       <c r="P62" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6988,7 +6994,7 @@
         <v>355</v>
       </c>
       <c r="P63" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7035,7 +7041,7 @@
         <v>355</v>
       </c>
       <c r="P64" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7082,7 +7088,7 @@
         <v>355</v>
       </c>
       <c r="P65" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7126,7 +7132,7 @@
         <v>355</v>
       </c>
       <c r="P66" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7173,7 +7179,7 @@
         <v>355</v>
       </c>
       <c r="P67" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7220,7 +7226,7 @@
         <v>355</v>
       </c>
       <c r="P68" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7267,7 +7273,7 @@
         <v>355</v>
       </c>
       <c r="P69" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7314,7 +7320,7 @@
         <v>355</v>
       </c>
       <c r="P70" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7358,7 +7364,7 @@
         <v>355</v>
       </c>
       <c r="P71" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7402,7 +7408,7 @@
         <v>355</v>
       </c>
       <c r="P72" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7449,7 +7455,7 @@
         <v>355</v>
       </c>
       <c r="P73" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7493,7 +7499,7 @@
         <v>355</v>
       </c>
       <c r="P74" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7537,7 +7543,7 @@
         <v>355</v>
       </c>
       <c r="P75" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7584,7 +7590,7 @@
         <v>355</v>
       </c>
       <c r="P76" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7628,7 +7634,7 @@
         <v>355</v>
       </c>
       <c r="P77" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7672,7 +7678,7 @@
         <v>355</v>
       </c>
       <c r="P78" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="79" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7719,7 +7725,7 @@
         <v>355</v>
       </c>
       <c r="P79" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="80" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7766,7 +7772,7 @@
         <v>355</v>
       </c>
       <c r="P80" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7810,7 +7816,7 @@
         <v>355</v>
       </c>
       <c r="P81" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7857,7 +7863,7 @@
         <v>355</v>
       </c>
       <c r="P82" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7904,7 +7910,7 @@
         <v>355</v>
       </c>
       <c r="P83" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7951,7 +7957,7 @@
         <v>355</v>
       </c>
       <c r="P84" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7998,7 +8004,7 @@
         <v>355</v>
       </c>
       <c r="P85" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8045,7 +8051,7 @@
         <v>355</v>
       </c>
       <c r="P86" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8089,7 +8095,7 @@
         <v>355</v>
       </c>
       <c r="P87" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8133,7 +8139,7 @@
         <v>355</v>
       </c>
       <c r="P88" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8177,7 +8183,7 @@
         <v>355</v>
       </c>
       <c r="P89" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8221,7 +8227,7 @@
         <v>355</v>
       </c>
       <c r="P90" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8268,7 +8274,7 @@
         <v>355</v>
       </c>
       <c r="P91" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8315,7 +8321,7 @@
         <v>355</v>
       </c>
       <c r="P92" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8362,7 +8368,7 @@
         <v>355</v>
       </c>
       <c r="P93" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="94" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8406,7 +8412,7 @@
         <v>355</v>
       </c>
       <c r="P94" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="95" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8453,7 +8459,7 @@
         <v>355</v>
       </c>
       <c r="P95" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="96" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8500,7 +8506,7 @@
         <v>355</v>
       </c>
       <c r="P96" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="97" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8547,7 +8553,7 @@
         <v>355</v>
       </c>
       <c r="P97" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="98" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8591,7 +8597,7 @@
         <v>355</v>
       </c>
       <c r="P98" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="99" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8635,7 +8641,7 @@
         <v>355</v>
       </c>
       <c r="P99" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8679,7 +8685,7 @@
         <v>355</v>
       </c>
       <c r="P100" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8723,7 +8729,7 @@
         <v>355</v>
       </c>
       <c r="P101" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="102" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8767,7 +8773,7 @@
         <v>355</v>
       </c>
       <c r="P102" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="103" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8814,7 +8820,7 @@
         <v>355</v>
       </c>
       <c r="P103" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8858,7 +8864,7 @@
         <v>355</v>
       </c>
       <c r="P104" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="105" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8905,7 +8911,7 @@
         <v>355</v>
       </c>
       <c r="P105" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="106" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8952,7 +8958,7 @@
         <v>355</v>
       </c>
       <c r="P106" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="107" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8999,7 +9005,7 @@
         <v>355</v>
       </c>
       <c r="P107" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="108" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9043,7 +9049,7 @@
         <v>355</v>
       </c>
       <c r="P108" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="109" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9087,7 +9093,7 @@
         <v>355</v>
       </c>
       <c r="P109" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="110" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9134,7 +9140,7 @@
         <v>355</v>
       </c>
       <c r="P110" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="111" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9178,7 +9184,7 @@
         <v>355</v>
       </c>
       <c r="P111" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="112" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9222,7 +9228,7 @@
         <v>355</v>
       </c>
       <c r="P112" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="113" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9266,7 +9272,7 @@
         <v>355</v>
       </c>
       <c r="P113" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="114" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9310,7 +9316,7 @@
         <v>355</v>
       </c>
       <c r="P114" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="115" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9354,7 +9360,7 @@
         <v>355</v>
       </c>
       <c r="P115" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="116" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9401,7 +9407,7 @@
         <v>355</v>
       </c>
       <c r="P116" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="117" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9445,7 +9451,7 @@
         <v>355</v>
       </c>
       <c r="P117" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="118" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9489,7 +9495,7 @@
         <v>355</v>
       </c>
       <c r="P118" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="119" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9533,7 +9539,7 @@
         <v>355</v>
       </c>
       <c r="P119" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="120" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9577,7 +9583,7 @@
         <v>355</v>
       </c>
       <c r="P120" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="121" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9627,7 +9633,7 @@
         <v>355</v>
       </c>
       <c r="P121" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="122" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9671,7 +9677,7 @@
         <v>355</v>
       </c>
       <c r="P122" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="123" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9718,7 +9724,7 @@
         <v>355</v>
       </c>
       <c r="P123" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="124" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9765,7 +9771,7 @@
         <v>355</v>
       </c>
       <c r="P124" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="125" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9809,7 +9815,7 @@
         <v>355</v>
       </c>
       <c r="P125" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="126" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9850,7 +9856,7 @@
         <v>355</v>
       </c>
       <c r="P126" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="127" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9891,7 +9897,7 @@
         <v>355</v>
       </c>
       <c r="P127" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="128" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9935,7 +9941,7 @@
         <v>355</v>
       </c>
       <c r="P128" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="129" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9979,7 +9985,7 @@
         <v>355</v>
       </c>
       <c r="P129" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="130" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10026,7 +10032,7 @@
         <v>355</v>
       </c>
       <c r="P130" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="131" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10070,7 +10076,7 @@
         <v>355</v>
       </c>
       <c r="P131" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="132" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10117,7 +10123,7 @@
         <v>355</v>
       </c>
       <c r="P132" t="s">
-        <v>355</v>
+        <v>782</v>
       </c>
     </row>
     <row r="133" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10161,7 +10167,7 @@
         <v>761</v>
       </c>
       <c r="P133" s="10" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
     <row r="134" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10205,7 +10211,7 @@
         <v>767</v>
       </c>
       <c r="P134" t="s">
-        <v>27</v>
+        <v>781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made GPO lowercase in data and adjusted code
</commit_message>
<xml_diff>
--- a/reception_analysis_data.xlsx
+++ b/reception_analysis_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah Zeldin\Documents\R stuff\R projects\dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7963798A-AA4D-4FD1-80ED-D467CBCB574D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEFD6DE-0FB3-4F8B-B398-EA7E774BB9A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{05090813-5714-498C-A2E7-B769A3723D8B}"/>
   </bookViews>
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="789">
   <si>
     <t>Article</t>
   </si>
@@ -3470,6 +3470,18 @@
   </si>
   <si>
     <t>incomplete</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -4021,7 +4033,7 @@
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4112,7 +4124,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>21</v>
@@ -4159,7 +4171,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>32</v>
@@ -4206,7 +4218,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>39</v>
@@ -4250,7 +4262,7 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>44</v>
@@ -4300,7 +4312,7 @@
         <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>44</v>
@@ -4350,7 +4362,7 @@
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>44</v>
@@ -4400,7 +4412,7 @@
         <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>44</v>
@@ -4447,7 +4459,7 @@
         <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>44</v>
@@ -4494,7 +4506,7 @@
         <v>84</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>44</v>
@@ -4541,7 +4553,7 @@
         <v>52</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>44</v>
@@ -4591,7 +4603,7 @@
         <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>44</v>
@@ -4638,7 +4650,7 @@
         <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>44</v>
@@ -4682,7 +4694,7 @@
         <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>108</v>
@@ -4729,7 +4741,7 @@
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>108</v>
@@ -4779,7 +4791,7 @@
         <v>84</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>121</v>
@@ -4823,7 +4835,7 @@
         <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>126</v>
@@ -4870,7 +4882,7 @@
         <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>132</v>
@@ -4917,7 +4929,7 @@
         <v>70</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>140</v>
@@ -4964,7 +4976,7 @@
         <v>70</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>140</v>
@@ -5011,7 +5023,7 @@
         <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>152</v>
@@ -5058,7 +5070,7 @@
         <v>19</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>152</v>
@@ -5105,7 +5117,7 @@
         <v>19</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>152</v>
@@ -5152,7 +5164,7 @@
         <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>140</v>
@@ -5199,7 +5211,7 @@
         <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>40</v>
@@ -5249,7 +5261,7 @@
         <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>185</v>
@@ -5296,7 +5308,7 @@
         <v>19</v>
       </c>
       <c r="G27" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>191</v>
@@ -5340,7 +5352,7 @@
         <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>195</v>
@@ -5387,7 +5399,7 @@
         <v>19</v>
       </c>
       <c r="G29" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>201</v>
@@ -5431,7 +5443,7 @@
         <v>70</v>
       </c>
       <c r="G30" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>207</v>
@@ -5478,7 +5490,7 @@
         <v>19</v>
       </c>
       <c r="G31" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>207</v>
@@ -5525,7 +5537,7 @@
         <v>19</v>
       </c>
       <c r="G32" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>219</v>
@@ -5572,7 +5584,7 @@
         <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>140</v>
@@ -5619,7 +5631,7 @@
         <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>233</v>
@@ -5666,7 +5678,7 @@
         <v>241</v>
       </c>
       <c r="G35" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>242</v>
@@ -5716,7 +5728,7 @@
         <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>251</v>
@@ -5763,7 +5775,7 @@
         <v>70</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>258</v>
@@ -5810,7 +5822,7 @@
         <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>265</v>
@@ -5860,7 +5872,7 @@
         <v>84</v>
       </c>
       <c r="G39" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>274</v>
@@ -5910,7 +5922,7 @@
         <v>281</v>
       </c>
       <c r="G40" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>274</v>
@@ -5960,7 +5972,7 @@
         <v>19</v>
       </c>
       <c r="G41" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>274</v>
@@ -6007,7 +6019,7 @@
         <v>70</v>
       </c>
       <c r="G42" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>291</v>
@@ -6054,7 +6066,7 @@
         <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>291</v>
@@ -6101,7 +6113,7 @@
         <v>70</v>
       </c>
       <c r="G44" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>302</v>
@@ -6148,7 +6160,7 @@
         <v>19</v>
       </c>
       <c r="G45" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>307</v>
@@ -6198,7 +6210,7 @@
         <v>70</v>
       </c>
       <c r="G46" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>307</v>
@@ -6245,7 +6257,7 @@
         <v>19</v>
       </c>
       <c r="G47" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>319</v>
@@ -6289,7 +6301,7 @@
         <v>19</v>
       </c>
       <c r="G48" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>326</v>
@@ -6336,7 +6348,7 @@
         <v>19</v>
       </c>
       <c r="G49" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>195</v>
@@ -6377,7 +6389,7 @@
         <v>19</v>
       </c>
       <c r="G50" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>338</v>
@@ -6421,7 +6433,7 @@
         <v>19</v>
       </c>
       <c r="G51" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>344</v>
@@ -6465,7 +6477,7 @@
         <v>52</v>
       </c>
       <c r="G52" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>351</v>
@@ -6509,7 +6521,7 @@
         <v>70</v>
       </c>
       <c r="G53" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>40</v>
@@ -6556,7 +6568,7 @@
         <v>366</v>
       </c>
       <c r="G54" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>367</v>
@@ -6603,7 +6615,7 @@
         <v>70</v>
       </c>
       <c r="G55" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>40</v>
@@ -6650,7 +6662,7 @@
         <v>19</v>
       </c>
       <c r="G56" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>40</v>
@@ -6694,7 +6706,7 @@
         <v>19</v>
       </c>
       <c r="G57" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>40</v>
@@ -6741,7 +6753,7 @@
         <v>52</v>
       </c>
       <c r="G58" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>40</v>
@@ -6788,7 +6800,7 @@
         <v>281</v>
       </c>
       <c r="G59" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>40</v>
@@ -6835,7 +6847,7 @@
         <v>397</v>
       </c>
       <c r="G60" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>40</v>
@@ -6882,7 +6894,7 @@
         <v>19</v>
       </c>
       <c r="G61" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>40</v>
@@ -6929,7 +6941,7 @@
         <v>70</v>
       </c>
       <c r="G62" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>40</v>
@@ -6976,7 +6988,7 @@
         <v>414</v>
       </c>
       <c r="G63" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>415</v>
@@ -7023,7 +7035,7 @@
         <v>52</v>
       </c>
       <c r="G64" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>40</v>
@@ -7070,7 +7082,7 @@
         <v>70</v>
       </c>
       <c r="G65" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>428</v>
@@ -7117,7 +7129,7 @@
         <v>366</v>
       </c>
       <c r="G66" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>40</v>
@@ -7161,7 +7173,7 @@
         <v>281</v>
       </c>
       <c r="G67" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>40</v>
@@ -7208,7 +7220,7 @@
         <v>414</v>
       </c>
       <c r="G68" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>40</v>
@@ -7255,7 +7267,7 @@
         <v>450</v>
       </c>
       <c r="G69" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>40</v>
@@ -7302,7 +7314,7 @@
         <v>19</v>
       </c>
       <c r="G70" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>455</v>
@@ -7349,7 +7361,7 @@
         <v>19</v>
       </c>
       <c r="G71" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>367</v>
@@ -7393,7 +7405,7 @@
         <v>19</v>
       </c>
       <c r="G72" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>463</v>
@@ -7437,7 +7449,7 @@
         <v>52</v>
       </c>
       <c r="G73" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>415</v>
@@ -7484,7 +7496,7 @@
         <v>52</v>
       </c>
       <c r="G74" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>472</v>
@@ -7528,7 +7540,7 @@
         <v>52</v>
       </c>
       <c r="G75" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>367</v>
@@ -7572,7 +7584,7 @@
         <v>483</v>
       </c>
       <c r="G76" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>351</v>
@@ -7619,7 +7631,7 @@
         <v>366</v>
       </c>
       <c r="G77" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>367</v>
@@ -7663,7 +7675,7 @@
         <v>366</v>
       </c>
       <c r="G78" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>351</v>
@@ -7707,7 +7719,7 @@
         <v>52</v>
       </c>
       <c r="G79" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>415</v>
@@ -7754,7 +7766,7 @@
         <v>52</v>
       </c>
       <c r="G80" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>499</v>
@@ -7801,7 +7813,7 @@
         <v>52</v>
       </c>
       <c r="G81" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>351</v>
@@ -7845,7 +7857,7 @@
         <v>70</v>
       </c>
       <c r="G82" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>511</v>
@@ -7892,7 +7904,7 @@
         <v>52</v>
       </c>
       <c r="G83" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>518</v>
@@ -7939,7 +7951,7 @@
         <v>281</v>
       </c>
       <c r="G84" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>351</v>
@@ -7986,7 +7998,7 @@
         <v>84</v>
       </c>
       <c r="G85" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>531</v>
@@ -8033,7 +8045,7 @@
         <v>366</v>
       </c>
       <c r="G86" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>351</v>
@@ -8080,7 +8092,7 @@
         <v>366</v>
       </c>
       <c r="G87" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>543</v>
@@ -8124,7 +8136,7 @@
         <v>366</v>
       </c>
       <c r="G88" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>415</v>
@@ -8168,7 +8180,7 @@
         <v>70</v>
       </c>
       <c r="G89" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>415</v>
@@ -8212,7 +8224,7 @@
         <v>483</v>
       </c>
       <c r="G90" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>367</v>
@@ -8256,7 +8268,7 @@
         <v>483</v>
       </c>
       <c r="G91" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>351</v>
@@ -8303,7 +8315,7 @@
         <v>366</v>
       </c>
       <c r="G92" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>367</v>
@@ -8350,7 +8362,7 @@
         <v>366</v>
       </c>
       <c r="G93" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>351</v>
@@ -8397,7 +8409,7 @@
         <v>70</v>
       </c>
       <c r="G94" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>428</v>
@@ -8441,7 +8453,7 @@
         <v>84</v>
       </c>
       <c r="G95" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>582</v>
@@ -8488,7 +8500,7 @@
         <v>70</v>
       </c>
       <c r="G96" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>351</v>
@@ -8535,7 +8547,7 @@
         <v>52</v>
       </c>
       <c r="G97" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>463</v>
@@ -8582,7 +8594,7 @@
         <v>70</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>600</v>
@@ -8626,7 +8638,7 @@
         <v>414</v>
       </c>
       <c r="G99" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>605</v>
@@ -8670,7 +8682,7 @@
         <v>70</v>
       </c>
       <c r="G100" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>600</v>
@@ -8714,7 +8726,7 @@
         <v>70</v>
       </c>
       <c r="G101" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>582</v>
@@ -8758,7 +8770,7 @@
         <v>84</v>
       </c>
       <c r="G102" s="5" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>600</v>
@@ -8802,7 +8814,7 @@
         <v>623</v>
       </c>
       <c r="G103" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>624</v>
@@ -8849,7 +8861,7 @@
         <v>70</v>
       </c>
       <c r="G104" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>630</v>
@@ -8893,7 +8905,7 @@
         <v>636</v>
       </c>
       <c r="G105" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>463</v>
@@ -8940,7 +8952,7 @@
         <v>70</v>
       </c>
       <c r="G106" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>428</v>
@@ -8987,7 +8999,7 @@
         <v>70</v>
       </c>
       <c r="G107" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>630</v>
@@ -9034,7 +9046,7 @@
         <v>650</v>
       </c>
       <c r="G108" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>351</v>
@@ -9078,7 +9090,7 @@
         <v>70</v>
       </c>
       <c r="G109" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>351</v>
@@ -9122,7 +9134,7 @@
         <v>52</v>
       </c>
       <c r="G110" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>351</v>
@@ -9169,7 +9181,7 @@
         <v>636</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>663</v>
@@ -9213,7 +9225,7 @@
         <v>19</v>
       </c>
       <c r="G112" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>351</v>
@@ -9257,7 +9269,7 @@
         <v>366</v>
       </c>
       <c r="G113" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>351</v>
@@ -9301,7 +9313,7 @@
         <v>52</v>
       </c>
       <c r="G114" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>463</v>
@@ -9345,7 +9357,7 @@
         <v>681</v>
       </c>
       <c r="G115" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>531</v>
@@ -9389,7 +9401,7 @@
         <v>681</v>
       </c>
       <c r="G116" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>684</v>
@@ -9436,7 +9448,7 @@
         <v>70</v>
       </c>
       <c r="G117" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>600</v>
@@ -9480,7 +9492,7 @@
         <v>52</v>
       </c>
       <c r="G118" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>351</v>
@@ -9524,7 +9536,7 @@
         <v>52</v>
       </c>
       <c r="G119" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>351</v>
@@ -9568,7 +9580,7 @@
         <v>70</v>
       </c>
       <c r="G120" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>511</v>
@@ -9612,7 +9624,7 @@
         <v>19</v>
       </c>
       <c r="G121" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>351</v>
@@ -9662,7 +9674,7 @@
         <v>52</v>
       </c>
       <c r="G122" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>351</v>
@@ -9706,7 +9718,7 @@
         <v>716</v>
       </c>
       <c r="G123" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>463</v>
@@ -9753,7 +9765,7 @@
         <v>70</v>
       </c>
       <c r="G124" t="s">
-        <v>70</v>
+        <v>788</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>722</v>
@@ -9800,7 +9812,7 @@
         <v>19</v>
       </c>
       <c r="G125" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>415</v>
@@ -9844,7 +9856,7 @@
         <v>19</v>
       </c>
       <c r="G126" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>415</v>
@@ -9885,7 +9897,7 @@
         <v>19</v>
       </c>
       <c r="G127" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>734</v>
@@ -9926,7 +9938,7 @@
         <v>19</v>
       </c>
       <c r="G128" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>531</v>
@@ -9970,7 +9982,7 @@
         <v>19</v>
       </c>
       <c r="G129" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H129" s="3" t="s">
         <v>740</v>
@@ -10014,7 +10026,7 @@
         <v>52</v>
       </c>
       <c r="G130" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>351</v>
@@ -10061,7 +10073,7 @@
         <v>52</v>
       </c>
       <c r="G131" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H131" s="3" t="s">
         <v>351</v>
@@ -10105,7 +10117,7 @@
         <v>84</v>
       </c>
       <c r="G132" t="s">
-        <v>85</v>
+        <v>787</v>
       </c>
       <c r="H132" t="s">
         <v>367</v>
@@ -10152,7 +10164,7 @@
         <v>281</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>53</v>
+        <v>786</v>
       </c>
       <c r="H133" s="12" t="s">
         <v>44</v>
@@ -10196,7 +10208,7 @@
         <v>19</v>
       </c>
       <c r="G134" t="s">
-        <v>20</v>
+        <v>785</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>764</v>

</xml_diff>